<commit_message>
plots for piecewise linear alpha parameter estimation
</commit_message>
<xml_diff>
--- a/heroin_parameter_estimation/heroin_model_multistart_with_quarters/final_results_piecewise/x_final_parameters_unrounded_piecewise.xlsx
+++ b/heroin_parameter_estimation/heroin_model_multistart_with_quarters/final_results_piecewise/x_final_parameters_unrounded_piecewise.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillips/Documents/Research/Heroin_model/heroin_parameter_estimation/heroin_model_multistart_with_quarters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillips/Documents/Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC0F5A6-1A2F-8B46-8041-4DE4520D4D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA0F3346-7396-824B-B0B5-25431D39EEA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16740" xr2:uid="{1E89FA12-A334-5847-99A1-CABB0881191B}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16740" xr2:uid="{8634B3A6-A971-5042-8555-3F1ADC8F9F7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,66 +370,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A8BA7E-B590-FB45-882E-3FCAF1D82984}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BDDAAD-0004-974F-9A23-40359D058225}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>-3.6540125984464702E-3</v>
+        <v>-4.83153360588449E-3</v>
       </c>
       <c r="B1">
-        <v>3.4420413147962098E-3</v>
-      </c>
-      <c r="C1" s="1">
-        <v>3.5339298324207099E-4</v>
-      </c>
-      <c r="D1" s="1">
-        <v>5.0041031618096202E-4</v>
+        <v>4.3976392776770403E-3</v>
+      </c>
+      <c r="C1">
+        <v>4.6859953972325599E-4</v>
+      </c>
+      <c r="D1">
+        <v>5.0177956562447905E-4</v>
       </c>
       <c r="E1">
-        <v>2.4970009615304498</v>
+        <v>2.4949598417671499</v>
       </c>
       <c r="F1">
-        <v>1.3495927564042499E-3</v>
+        <v>1.4578030368749401E-3</v>
       </c>
       <c r="G1">
-        <v>0.141992169886001</v>
+        <v>0.148273757923292</v>
       </c>
       <c r="H1">
-        <v>7.7080830501723901E-2</v>
+        <v>2.83184279154154E-2</v>
       </c>
       <c r="I1">
-        <v>0.32846768251128</v>
+        <v>0.31805886328147598</v>
       </c>
       <c r="J1">
-        <v>0.121471313211613</v>
+        <v>2.3790760445498602</v>
       </c>
       <c r="K1">
-        <v>4.5782446786908897E-2</v>
+        <v>4.8152163179444402E-2</v>
       </c>
       <c r="L1">
-        <v>0.26909381236535901</v>
+        <v>0.28312955275417001</v>
       </c>
       <c r="M1">
-        <v>9.7068107086103E-2</v>
+        <v>9.4988976008938505E-2</v>
       </c>
       <c r="N1">
-        <v>6.4522477435450696E-3</v>
-      </c>
-      <c r="O1" s="1">
-        <v>8.4707519808550804E-4</v>
+        <v>6.4652335336897399E-3</v>
+      </c>
+      <c r="O1">
+        <v>8.4279137833710596E-4</v>
       </c>
       <c r="P1">
-        <v>2.19656279519325E-2</v>
+        <v>5.8439378633657599E-2</v>
       </c>
       <c r="Q1">
-        <v>-2.9892750551276E-2</v>
+        <v>-3.1298273617099498E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>